<commit_message>
add the concept map
</commit_message>
<xml_diff>
--- a/output/ValueSet-option-set-yes-no.xlsx
+++ b/output/ValueSet-option-set-yes-no.xlsx
@@ -8,15 +8,12 @@
   <sheets>
     <sheet name="Metadata" r:id="rId3" sheetId="1"/>
     <sheet name="Include #0" r:id="rId4" sheetId="2"/>
-    <sheet name="Include #1" r:id="rId5" sheetId="3"/>
-    <sheet name="Include #2" r:id="rId6" sheetId="4"/>
-    <sheet name="Include #3" r:id="rId7" sheetId="5"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
   <si>
     <t>Property</t>
   </si>
@@ -45,7 +42,7 @@
     <t>Title</t>
   </si>
   <si>
-    <t>Option Set - Yes / No / Yes-only / Don't know / Not applicable / Positive / Negative</t>
+    <t>Option Set - Yes / No / Yes-only / Don't know / Not applicable</t>
   </si>
   <si>
     <t>Status</t>
@@ -63,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-09-04T17:51:26+05:45</t>
+    <t>2025-09-04T23:57:58+05:45</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -90,8 +87,7 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Master option set for Yes/No/Yes-only/Don't know/Not applicable, Positive/Negative questions, including Nepali designations:छ/छैन, 
-हो/होइन, गराएको/नगराएको, लिएको/नलिएको, भएको/नभएको, पास/फेल, पाएको/नपाएको
+    <t xml:space="preserve">Master option set for Yes/No/Yes-only/Don't know/Not applicable, including Nepali designations:छ/छैन, हो/होइन, गराएको/नगराएको, लिएको/नलिएको, भएको/नभएको, पाएको/नपाएको
 Used for:
 - Presumptive TB Case (सम्भावित क्षयरोग विरामी)
 - Gender Based Violence (लैंगिक हिंसा)
@@ -102,7 +98,12 @@
 - Stridor (Yes only)
 - Wheezing (Yes only)
 - Condom Use
-- Lab test results (Positive/Negative)</t>
+- Lab test results (Positive/Negative)
+| HL7 v2-0532 Code | SNOMED CT Code | English Meaning       | Nepali Variants                                      |
+|-----------------|----------------|--------------------|-----------------------------------------------------|
+| Y               | 373066001      | Yes / Affirmative  | हो / गराएको / लिएको / भएको / पाएको              |
+| N               | 373067005      | No / Negative      | होइन / नगराएको / नलिएको / नभएको / नपाएको      |
+</t>
   </si>
   <si>
     <t>Purpose</t>
@@ -120,43 +121,10 @@
     <t>BooleanType[null]</t>
   </si>
   <si>
-    <t>Concept</t>
-  </si>
-  <si>
-    <t>373066001</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>373067005</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>373068000</t>
-  </si>
-  <si>
-    <t>Don't know</t>
-  </si>
-  <si>
-    <t>373069008</t>
-  </si>
-  <si>
-    <t>Not applicable</t>
-  </si>
-  <si>
-    <t>10828004</t>
-  </si>
-  <si>
-    <t>Positive</t>
-  </si>
-  <si>
-    <t>260385009</t>
-  </si>
-  <si>
-    <t>Negative</t>
+    <t>Codes</t>
+  </si>
+  <si>
+    <t>All codes</t>
   </si>
   <si>
     <t/>
@@ -165,43 +133,7 @@
     <t>System URI</t>
   </si>
   <si>
-    <t>http://snomed.info/sct</t>
-  </si>
-  <si>
-    <t>yes</t>
-  </si>
-  <si>
-    <t>no</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>https://fhir.hmis.gov.np/CodeSystem/yes-no</t>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>UNK</t>
-  </si>
-  <si>
-    <t>Unknown</t>
-  </si>
-  <si>
-    <t>NA</t>
-  </si>
-  <si>
     <t>http://terminology.hl7.org/CodeSystem/v2-0532</t>
-  </si>
-  <si>
-    <t>Yes only</t>
   </si>
 </sst>
 </file>
@@ -478,241 +410,6 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
-  <cols>
-    <col min="1" max="1" width="30.703125" customWidth="true"/>
-    <col min="2" max="2" width="50.703125" customWidth="true"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s" s="1">
-        <v>30</v>
-      </c>
-      <c r="B1" t="s" s="1">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s" s="2">
-        <v>31</v>
-      </c>
-      <c r="B2" t="s" s="2">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s" s="2">
-        <v>33</v>
-      </c>
-      <c r="B3" t="s" s="2">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="B4" t="s" s="2">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="B5" t="s" s="2">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="B6" t="s" s="2">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="B7" t="s" s="2">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="B8" t="s" s="2">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="B9" t="s" s="2">
-        <v>45</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
-  <cols>
-    <col min="1" max="1" width="30.703125" customWidth="true"/>
-    <col min="2" max="2" width="50.703125" customWidth="true"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s" s="1">
-        <v>30</v>
-      </c>
-      <c r="B1" t="s" s="1">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="B2" t="s" s="2">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s" s="2">
-        <v>47</v>
-      </c>
-      <c r="B3" t="s" s="2">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="B4" t="s" s="2">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s" s="2">
-        <v>49</v>
-      </c>
-      <c r="B5" t="s" s="2">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="B6" t="s" s="2">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="B7" t="s" s="2">
-        <v>50</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
-  <cols>
-    <col min="1" max="1" width="30.703125" customWidth="true"/>
-    <col min="2" max="2" width="50.703125" customWidth="true"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s" s="1">
-        <v>30</v>
-      </c>
-      <c r="B1" t="s" s="1">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s" s="2">
-        <v>51</v>
-      </c>
-      <c r="B2" t="s" s="2">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s" s="2">
-        <v>52</v>
-      </c>
-      <c r="B3" t="s" s="2">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s" s="2">
-        <v>53</v>
-      </c>
-      <c r="B4" t="s" s="2">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s" s="2">
-        <v>55</v>
-      </c>
-      <c r="B5" t="s" s="2">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="B6" t="s" s="2">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="B7" t="s" s="2">
-        <v>56</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -727,32 +424,26 @@
       <c r="A1" t="s" s="1">
         <v>30</v>
       </c>
-      <c r="B1" t="s" s="1">
-        <v>23</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="B2" t="s" s="2">
-        <v>57</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="2">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="B3" t="s" s="2">
-        <v>43</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="2">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="B4" t="s" s="2">
-        <v>50</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>